<commit_message>
Aplicacao realiza a leitura do arquivo excel e verifica se no diretorio existe o atendimento.
</commit_message>
<xml_diff>
--- a/ServerCleaner V2/Novo(a) Planilha do Microsoft Excel.xlsx
+++ b/ServerCleaner V2/Novo(a) Planilha do Microsoft Excel.xlsx
@@ -14,68 +14,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Valores</t>
-  </si>
-  <si>
-    <t>Valores1</t>
-  </si>
-  <si>
-    <t>Valores3</t>
-  </si>
-  <si>
-    <t>Valores4</t>
-  </si>
-  <si>
-    <t>Valores5</t>
-  </si>
-  <si>
-    <t>Valores6</t>
-  </si>
-  <si>
-    <t>Valores7</t>
-  </si>
-  <si>
-    <t>Valores8</t>
-  </si>
-  <si>
-    <t>Valores9</t>
-  </si>
-  <si>
-    <t>Valores10</t>
-  </si>
-  <si>
-    <t>Valores11</t>
-  </si>
-  <si>
-    <t>Valores12</t>
-  </si>
-  <si>
-    <t>Linha/Coluna</t>
-  </si>
-  <si>
-    <t>Coluna 1</t>
-  </si>
-  <si>
-    <t>Coluna 2</t>
-  </si>
-  <si>
-    <t>Coluna 3</t>
-  </si>
-  <si>
-    <t>Valores2</t>
-  </si>
-  <si>
-    <t>Valores13</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Canal</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>RN-DIREÇÃO</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Módulo</t>
+  </si>
+  <si>
+    <t>Data Abertura</t>
+  </si>
+  <si>
+    <t>Atendente</t>
+  </si>
+  <si>
+    <t>Problema</t>
+  </si>
+  <si>
+    <t>Data Solução</t>
+  </si>
+  <si>
+    <t>Solução</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>Posição</t>
+  </si>
+  <si>
+    <t>Estágio</t>
+  </si>
+  <si>
+    <t>Visitas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,82 +415,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>8349930</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>8354433</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>